<commit_message>
add nayak2014 and lalisseAsudeh2015
</commit_message>
<xml_diff>
--- a/stimuli/resources/LalliseAsudeh2015_adjective-intersectivity.xlsx
+++ b/stimuli/resources/LalliseAsudeh2015_adjective-intersectivity.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C8793C-8243-BC4D-888F-180450104FDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="14680" yWindow="5100" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14685" yWindow="5100" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$301</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$301</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="311">
   <si>
     <t>short</t>
   </si>
@@ -950,12 +949,18 @@
   </si>
   <si>
     <t>tag3</t>
+  </si>
+  <si>
+    <t>subsective</t>
+  </si>
+  <si>
+    <t>select</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -979,12 +984,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -999,12 +1010,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1286,17 +1300,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:D301"/>
+  <dimension ref="A1:E301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E295" sqref="E295"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A302" sqref="A302"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>305</v>
       </c>
@@ -1309,8 +1326,11 @@
       <c r="D1" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1321,8 +1341,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
@@ -1331,8 +1351,11 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1343,8 +1366,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
@@ -1353,8 +1376,11 @@
       <c r="C5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1362,7 +1388,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1370,7 +1396,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1381,7 +1407,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -1392,7 +1418,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -1403,7 +1429,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -1414,7 +1440,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -1425,7 +1451,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -1436,7 +1462,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -1450,7 +1476,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -1458,7 +1484,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -1469,7 +1495,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -1477,7 +1503,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
@@ -1485,7 +1511,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
@@ -1493,7 +1519,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
@@ -1501,7 +1527,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
@@ -1509,7 +1535,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -1520,7 +1546,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
@@ -1528,7 +1554,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
@@ -1536,8 +1562,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B25" t="s">
@@ -1546,8 +1572,11 @@
       <c r="C25" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="E25" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
@@ -1558,7 +1587,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>30</v>
       </c>
@@ -1569,7 +1598,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
@@ -1580,7 +1609,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>32</v>
       </c>
@@ -1588,7 +1617,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>33</v>
       </c>
@@ -1596,7 +1625,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>34</v>
       </c>
@@ -1604,7 +1633,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>35</v>
       </c>
@@ -1612,8 +1641,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B33" t="s">
@@ -1622,8 +1651,11 @@
       <c r="C33" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="E33" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>37</v>
       </c>
@@ -1634,7 +1666,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>38</v>
       </c>
@@ -1645,7 +1677,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>39</v>
       </c>
@@ -1656,7 +1688,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>40</v>
       </c>
@@ -1664,7 +1696,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>41</v>
       </c>
@@ -1675,7 +1707,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>42</v>
       </c>
@@ -1683,7 +1715,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>43</v>
       </c>
@@ -1691,7 +1723,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>44</v>
       </c>
@@ -1702,7 +1734,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>45</v>
       </c>
@@ -1710,7 +1742,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>46</v>
       </c>
@@ -1721,7 +1753,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>47</v>
       </c>
@@ -1729,7 +1761,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>48</v>
       </c>
@@ -1740,7 +1772,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>49</v>
       </c>
@@ -1751,7 +1783,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>50</v>
       </c>
@@ -1762,7 +1794,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>51</v>
       </c>
@@ -1770,7 +1802,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>52</v>
       </c>
@@ -1781,7 +1813,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>53</v>
       </c>
@@ -1789,7 +1821,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>54</v>
       </c>
@@ -1800,7 +1832,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>55</v>
       </c>
@@ -1808,8 +1840,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
+    <row r="53" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
         <v>56</v>
       </c>
       <c r="B53" t="s">
@@ -1818,8 +1850,11 @@
       <c r="C53" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E53" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>57</v>
       </c>
@@ -1830,7 +1865,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>58</v>
       </c>
@@ -1841,7 +1876,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>59</v>
       </c>
@@ -1849,7 +1884,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>60</v>
       </c>
@@ -1860,7 +1895,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>61</v>
       </c>
@@ -1871,7 +1906,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>62</v>
       </c>
@@ -1879,7 +1914,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>63</v>
       </c>
@@ -1890,7 +1925,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>64</v>
       </c>
@@ -1904,7 +1939,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>65</v>
       </c>
@@ -1912,7 +1947,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>66</v>
       </c>
@@ -1926,7 +1961,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>67</v>
       </c>
@@ -1937,7 +1972,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>68</v>
       </c>
@@ -1945,7 +1980,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>69</v>
       </c>
@@ -1953,7 +1988,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>70</v>
       </c>
@@ -1961,7 +1996,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>71</v>
       </c>
@@ -1972,7 +2007,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>72</v>
       </c>
@@ -1980,7 +2015,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>73</v>
       </c>
@@ -1991,7 +2026,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>74</v>
       </c>
@@ -1999,7 +2034,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>75</v>
       </c>
@@ -2010,7 +2045,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>76</v>
       </c>
@@ -2021,7 +2056,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>77</v>
       </c>
@@ -2029,15 +2064,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
+    <row r="75" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
         <v>78</v>
       </c>
       <c r="B75" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="E75" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>79</v>
       </c>
@@ -2048,7 +2086,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>80</v>
       </c>
@@ -2056,7 +2094,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>81</v>
       </c>
@@ -2067,15 +2105,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
+    <row r="79" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
         <v>82</v>
       </c>
       <c r="B79" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="E79" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>83</v>
       </c>
@@ -2083,7 +2124,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>84</v>
       </c>
@@ -2091,7 +2132,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>85</v>
       </c>
@@ -2099,7 +2140,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>86</v>
       </c>
@@ -2110,7 +2151,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>87</v>
       </c>
@@ -2118,7 +2159,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>88</v>
       </c>
@@ -2129,7 +2170,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>89</v>
       </c>
@@ -2137,7 +2178,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>90</v>
       </c>
@@ -2148,7 +2189,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>91</v>
       </c>
@@ -2159,7 +2200,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>92</v>
       </c>
@@ -2167,7 +2208,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>93</v>
       </c>
@@ -2178,7 +2219,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>94</v>
       </c>
@@ -2186,7 +2227,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>95</v>
       </c>
@@ -2194,7 +2235,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>96</v>
       </c>
@@ -2202,7 +2243,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>98</v>
       </c>
@@ -2210,7 +2251,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>99</v>
       </c>
@@ -2221,7 +2262,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>100</v>
       </c>
@@ -2229,7 +2270,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>101</v>
       </c>
@@ -2240,7 +2281,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>102</v>
       </c>
@@ -2248,7 +2289,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>103</v>
       </c>
@@ -2259,7 +2300,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>104</v>
       </c>
@@ -2270,7 +2311,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>105</v>
       </c>
@@ -2281,7 +2322,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>106</v>
       </c>
@@ -2295,7 +2336,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>107</v>
       </c>
@@ -2306,7 +2347,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>108</v>
       </c>
@@ -2314,7 +2355,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>109</v>
       </c>
@@ -2322,7 +2363,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>110</v>
       </c>
@@ -2330,7 +2371,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>111</v>
       </c>
@@ -2341,7 +2382,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>112</v>
       </c>
@@ -2349,7 +2390,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>113</v>
       </c>
@@ -2360,7 +2401,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>114</v>
       </c>
@@ -2371,15 +2412,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A111" s="1" t="s">
+    <row r="111" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A111" s="3" t="s">
         <v>115</v>
       </c>
       <c r="B111" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E111" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>116</v>
       </c>
@@ -2387,7 +2431,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>117</v>
       </c>
@@ -2398,7 +2442,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>118</v>
       </c>
@@ -2409,7 +2453,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>119</v>
       </c>
@@ -2417,7 +2461,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>120</v>
       </c>
@@ -2428,7 +2472,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>121</v>
       </c>
@@ -2436,7 +2480,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>122</v>
       </c>
@@ -2450,8 +2494,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A119" s="1" t="b">
+    <row r="119" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A119" s="3" t="b">
         <v>1</v>
       </c>
       <c r="B119" t="s">
@@ -2460,8 +2504,11 @@
       <c r="C119" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E119" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>123</v>
       </c>
@@ -2472,7 +2519,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>124</v>
       </c>
@@ -2480,7 +2527,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>125</v>
       </c>
@@ -2491,7 +2538,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>126</v>
       </c>
@@ -2502,7 +2549,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>127</v>
       </c>
@@ -2513,7 +2560,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>128</v>
       </c>
@@ -2524,7 +2571,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>129</v>
       </c>
@@ -2532,7 +2579,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>130</v>
       </c>
@@ -2543,7 +2590,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>131</v>
       </c>
@@ -2554,7 +2601,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>132</v>
       </c>
@@ -2562,7 +2609,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>133</v>
       </c>
@@ -2570,7 +2617,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>134</v>
       </c>
@@ -2578,7 +2625,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>135</v>
       </c>
@@ -2589,7 +2636,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>136</v>
       </c>
@@ -2597,7 +2644,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>137</v>
       </c>
@@ -2608,7 +2655,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>138</v>
       </c>
@@ -2616,7 +2663,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>139</v>
       </c>
@@ -2624,15 +2671,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A137" s="1" t="s">
+    <row r="137" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A137" s="3" t="s">
         <v>140</v>
       </c>
       <c r="B137" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="E137" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>141</v>
       </c>
@@ -2643,7 +2693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>142</v>
       </c>
@@ -2651,15 +2701,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A140" s="1" t="s">
+    <row r="140" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A140" s="3" t="s">
         <v>143</v>
       </c>
       <c r="B140" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="E140" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>144</v>
       </c>
@@ -2670,7 +2723,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>145</v>
       </c>
@@ -2678,15 +2731,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A143" s="1" t="s">
+    <row r="143" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A143" s="3" t="s">
         <v>146</v>
       </c>
       <c r="B143" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="E143" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>147</v>
       </c>
@@ -2697,7 +2753,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>148</v>
       </c>
@@ -2705,7 +2761,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="146" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>149</v>
       </c>
@@ -2716,7 +2772,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>150</v>
       </c>
@@ -2724,7 +2780,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="148" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>151</v>
       </c>
@@ -2735,7 +2791,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="149" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>152</v>
       </c>
@@ -2743,7 +2799,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="150" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>153</v>
       </c>
@@ -2751,7 +2807,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="151" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>154</v>
       </c>
@@ -2759,7 +2815,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="152" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>155</v>
       </c>
@@ -2770,7 +2826,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="153" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>156</v>
       </c>
@@ -2778,8 +2834,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="154" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A154" s="1" t="s">
+    <row r="154" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A154" s="3" t="s">
         <v>157</v>
       </c>
       <c r="B154" t="s">
@@ -2788,8 +2844,11 @@
       <c r="C154" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="155" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="E154" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>158</v>
       </c>
@@ -2797,7 +2856,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>159</v>
       </c>
@@ -2805,7 +2864,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>160</v>
       </c>
@@ -2813,7 +2872,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>161</v>
       </c>
@@ -2824,7 +2883,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="159" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>162</v>
       </c>
@@ -2832,7 +2891,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="160" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>163</v>
       </c>
@@ -2840,7 +2899,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>164</v>
       </c>
@@ -2848,7 +2907,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>165</v>
       </c>
@@ -2856,7 +2915,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="163" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>166</v>
       </c>
@@ -2864,7 +2923,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>167</v>
       </c>
@@ -2872,7 +2931,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="165" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>168</v>
       </c>
@@ -2883,7 +2942,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="166" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>169</v>
       </c>
@@ -2891,7 +2950,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="167" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>170</v>
       </c>
@@ -2899,7 +2958,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="168" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>171</v>
       </c>
@@ -2907,7 +2966,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="169" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>172</v>
       </c>
@@ -2915,7 +2974,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="170" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>173</v>
       </c>
@@ -2923,7 +2982,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="171" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>174</v>
       </c>
@@ -2934,7 +2993,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="172" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>175</v>
       </c>
@@ -2945,7 +3004,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="173" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>176</v>
       </c>
@@ -2956,7 +3015,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="174" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>177</v>
       </c>
@@ -2964,7 +3023,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="175" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>178</v>
       </c>
@@ -2975,7 +3034,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="176" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>179</v>
       </c>
@@ -2983,7 +3042,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="177" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>180</v>
       </c>
@@ -2991,8 +3050,8 @@
         <v>97</v>
       </c>
     </row>
-    <row r="178" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A178" s="1" t="s">
+    <row r="178" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A178" s="3" t="s">
         <v>181</v>
       </c>
       <c r="B178" t="s">
@@ -3001,8 +3060,11 @@
       <c r="C178" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="179" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="E178" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>182</v>
       </c>
@@ -3013,7 +3075,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="180" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>183</v>
       </c>
@@ -3021,7 +3083,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="181" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>184</v>
       </c>
@@ -3032,7 +3094,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="182" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>185</v>
       </c>
@@ -3043,7 +3105,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="183" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>186</v>
       </c>
@@ -3051,7 +3113,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="184" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>187</v>
       </c>
@@ -3059,7 +3121,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="185" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>188</v>
       </c>
@@ -3070,7 +3132,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="186" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>189</v>
       </c>
@@ -3081,7 +3143,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="187" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>190</v>
       </c>
@@ -3092,7 +3154,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="188" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>191</v>
       </c>
@@ -3100,7 +3162,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="189" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>192</v>
       </c>
@@ -3111,7 +3173,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="190" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>193</v>
       </c>
@@ -3119,7 +3181,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="191" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>194</v>
       </c>
@@ -3127,7 +3189,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="192" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>195</v>
       </c>
@@ -3135,7 +3197,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="193" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>196</v>
       </c>
@@ -3146,7 +3208,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="194" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>197</v>
       </c>
@@ -3154,7 +3216,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="195" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>198</v>
       </c>
@@ -3165,7 +3227,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="196" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>199</v>
       </c>
@@ -3173,7 +3235,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="197" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>200</v>
       </c>
@@ -3181,7 +3243,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="198" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>201</v>
       </c>
@@ -3189,7 +3251,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="199" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>202</v>
       </c>
@@ -3197,7 +3259,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="200" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>203</v>
       </c>
@@ -3205,7 +3267,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="201" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>204</v>
       </c>
@@ -3216,7 +3278,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="202" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>205</v>
       </c>
@@ -3224,7 +3286,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="203" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>206</v>
       </c>
@@ -3232,7 +3294,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="204" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>207</v>
       </c>
@@ -3240,7 +3302,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="205" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>208</v>
       </c>
@@ -3248,7 +3310,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="206" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>209</v>
       </c>
@@ -3256,7 +3318,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="207" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>210</v>
       </c>
@@ -3264,7 +3326,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="208" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>211</v>
       </c>
@@ -3272,7 +3334,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="209" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>212</v>
       </c>
@@ -3280,7 +3342,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="210" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>213</v>
       </c>
@@ -3288,7 +3350,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="211" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>214</v>
       </c>
@@ -3296,7 +3358,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="212" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>215</v>
       </c>
@@ -3304,7 +3366,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="213" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>216</v>
       </c>
@@ -3312,15 +3374,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="214" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A214" s="1" t="s">
+    <row r="214" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A214" s="3" t="s">
         <v>217</v>
       </c>
       <c r="B214" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="215" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="E214" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>218</v>
       </c>
@@ -3331,7 +3396,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="216" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>219</v>
       </c>
@@ -3339,7 +3404,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="217" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>220</v>
       </c>
@@ -3350,7 +3415,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="218" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>221</v>
       </c>
@@ -3358,7 +3423,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="219" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>222</v>
       </c>
@@ -3366,7 +3431,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="220" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>223</v>
       </c>
@@ -3377,7 +3442,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="221" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>224</v>
       </c>
@@ -3385,7 +3450,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="222" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>225</v>
       </c>
@@ -3393,7 +3458,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="223" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>226</v>
       </c>
@@ -3404,8 +3469,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="224" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A224" s="1" t="s">
+    <row r="224" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A224" s="3" t="s">
         <v>227</v>
       </c>
       <c r="B224" t="s">
@@ -3414,8 +3479,11 @@
       <c r="C224" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="225" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="E224" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>228</v>
       </c>
@@ -3423,7 +3491,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="226" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>229</v>
       </c>
@@ -3431,7 +3499,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="227" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>230</v>
       </c>
@@ -3439,7 +3507,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="228" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>231</v>
       </c>
@@ -3447,7 +3515,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="229" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>232</v>
       </c>
@@ -3455,7 +3523,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="230" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>233</v>
       </c>
@@ -3466,7 +3534,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="231" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
         <v>234</v>
       </c>
@@ -3474,7 +3542,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="232" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>235</v>
       </c>
@@ -3482,7 +3550,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="233" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
         <v>236</v>
       </c>
@@ -3493,7 +3561,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="234" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>237</v>
       </c>
@@ -3501,7 +3569,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="235" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
         <v>238</v>
       </c>
@@ -3509,7 +3577,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="236" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>239</v>
       </c>
@@ -3517,7 +3585,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="237" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
         <v>240</v>
       </c>
@@ -3528,7 +3596,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="238" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>241</v>
       </c>
@@ -3536,15 +3604,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="239" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A239" s="1" t="s">
+    <row r="239" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A239" s="3" t="s">
         <v>242</v>
       </c>
       <c r="B239" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="240" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="E239" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>243</v>
       </c>
@@ -3552,7 +3623,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="241" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
         <v>244</v>
       </c>
@@ -3560,7 +3631,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="242" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>245</v>
       </c>
@@ -3568,23 +3639,29 @@
         <v>2</v>
       </c>
     </row>
-    <row r="243" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A243" s="1" t="s">
+    <row r="243" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A243" s="3" t="s">
         <v>246</v>
       </c>
       <c r="B243" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="244" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A244" s="1" t="s">
+      <c r="E243" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A244" s="3" t="s">
         <v>247</v>
       </c>
       <c r="B244" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="245" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="E244" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>249</v>
       </c>
@@ -3595,7 +3672,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="246" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>250</v>
       </c>
@@ -3603,7 +3680,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="247" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
         <v>251</v>
       </c>
@@ -3611,7 +3688,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="248" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>252</v>
       </c>
@@ -3622,7 +3699,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="249" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
         <v>253</v>
       </c>
@@ -3630,7 +3707,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="250" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>254</v>
       </c>
@@ -3638,7 +3715,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="251" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>255</v>
       </c>
@@ -3646,7 +3723,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="252" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>256</v>
       </c>
@@ -3654,7 +3731,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="253" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>257</v>
       </c>
@@ -3665,7 +3742,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="254" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>258</v>
       </c>
@@ -3673,7 +3750,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="255" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
         <v>259</v>
       </c>
@@ -3684,7 +3761,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="256" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>260</v>
       </c>
@@ -3695,7 +3772,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="257" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
         <v>261</v>
       </c>
@@ -3706,7 +3783,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="258" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>262</v>
       </c>
@@ -3714,7 +3791,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="259" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
         <v>263</v>
       </c>
@@ -3722,7 +3799,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="260" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>264</v>
       </c>
@@ -3730,7 +3807,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="261" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
         <v>265</v>
       </c>
@@ -3741,7 +3818,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="262" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>266</v>
       </c>
@@ -3752,7 +3829,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="263" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
         <v>267</v>
       </c>
@@ -3763,7 +3840,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="264" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>268</v>
       </c>
@@ -3774,7 +3851,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="265" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
         <v>269</v>
       </c>
@@ -3782,7 +3859,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="266" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>270</v>
       </c>
@@ -3796,7 +3873,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="267" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
         <v>271</v>
       </c>
@@ -3804,7 +3881,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="268" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
         <v>272</v>
       </c>
@@ -3815,7 +3892,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="269" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
         <v>273</v>
       </c>
@@ -3823,7 +3900,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="270" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
         <v>274</v>
       </c>
@@ -3831,7 +3908,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="271" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
         <v>275</v>
       </c>
@@ -3839,7 +3916,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="272" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
         <v>276</v>
       </c>
@@ -3847,7 +3924,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="273" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
         <v>277</v>
       </c>
@@ -3855,7 +3932,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="274" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
         <v>278</v>
       </c>
@@ -3863,7 +3940,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="275" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
         <v>279</v>
       </c>
@@ -3871,7 +3948,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="276" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
         <v>280</v>
       </c>
@@ -3882,7 +3959,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="277" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
         <v>281</v>
       </c>
@@ -3890,7 +3967,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="278" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
         <v>282</v>
       </c>
@@ -3898,7 +3975,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="279" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
         <v>283</v>
       </c>
@@ -3906,7 +3983,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="280" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
         <v>284</v>
       </c>
@@ -3917,7 +3994,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="281" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
         <v>285</v>
       </c>
@@ -3925,7 +4002,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="282" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
         <v>286</v>
       </c>
@@ -3933,7 +4010,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="283" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
         <v>287</v>
       </c>
@@ -3941,7 +4018,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="284" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
         <v>288</v>
       </c>
@@ -3949,7 +4026,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="285" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
         <v>289</v>
       </c>
@@ -3960,7 +4037,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="286" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
         <v>290</v>
       </c>
@@ -3971,7 +4048,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="287" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
         <v>291</v>
       </c>
@@ -3979,7 +4056,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="288" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
         <v>292</v>
       </c>
@@ -3987,7 +4064,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="289" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
         <v>293</v>
       </c>
@@ -3995,7 +4072,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="290" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
         <v>294</v>
       </c>
@@ -4003,7 +4080,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="291" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
         <v>295</v>
       </c>
@@ -4011,7 +4088,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="292" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
         <v>296</v>
       </c>
@@ -4019,7 +4096,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="293" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
         <v>297</v>
       </c>
@@ -4027,7 +4104,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="294" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
         <v>298</v>
       </c>
@@ -4035,7 +4112,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="295" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
         <v>299</v>
       </c>
@@ -4046,7 +4123,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="296" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
         <v>300</v>
       </c>
@@ -4054,7 +4131,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="297" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
         <v>301</v>
       </c>
@@ -4062,7 +4139,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="298" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
         <v>302</v>
       </c>
@@ -4070,7 +4147,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="299" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
         <v>303</v>
       </c>
@@ -4078,7 +4155,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="300" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300" s="1" t="s">
         <v>304</v>
       </c>
@@ -4086,7 +4163,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>248</v>
       </c>
@@ -4095,24 +4172,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D301" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="N"/>
-        <filter val="Pw"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters blank="1">
-        <filter val="N"/>
-        <filter val="Pw"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="3">
-      <filters blank="1">
-        <filter val="N"/>
-        <filter val="Pw"/>
-      </filters>
+  <autoFilter ref="A1:E301">
+    <filterColumn colId="4">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>